<commit_message>
j'ai corrigé mes code pour deplacmment objet en bas et a gouche et droitt
</commit_message>
<xml_diff>
--- a/Docs/planification-Projet-Hanieh Mohajerani.xlsx
+++ b/Docs/planification-Projet-Hanieh Mohajerani.xlsx
@@ -5,12 +5,12 @@
   <workbookPr updateLinks="never" codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\cours\Semestre 1-2\Projet-Module-C#\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Cours-Semestre\Semestres\Semestre 1-2\Projet-Module-C#\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:11_{F44B1B77-61C4-4CD7-842C-3F7D4066D1F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDC79EB8-B8AE-43B0-8A6C-84A863302498}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Donnees" sheetId="7" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="78">
   <si>
     <t>Module :</t>
   </si>
@@ -268,7 +268,40 @@
     <t>j'ai fait le planification pour durée de travail</t>
   </si>
   <si>
-    <t>j'ai creé les methodes et la class  Vecteur2d et la classe SpaceShip et la methode DrawImage</t>
+    <t>créer git hub</t>
+  </si>
+  <si>
+    <t>j'ai créé mon git hub</t>
+  </si>
+  <si>
+    <t>j'ai creé les methodes et la class  Vecteur2d et la classe SpaceShip,classe game ,ballequitombe et gameobjet et ses methodes dedans</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> depelacer le jeu vers le bas </t>
+  </si>
+  <si>
+    <t>depelacer le jeu a gouche et droit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">j'ai ajouter un champ playerShip de type SpaceShip </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ajoutez le nouveau vaisseau à la liste des objets du jeu.</t>
+  </si>
+  <si>
+    <t>s la méthode Update de la classe SpaceShip</t>
+  </si>
+  <si>
+    <t>j'ai corrigé les codes et ca march,il va a gouche et droit juste.</t>
+  </si>
+  <si>
+    <t>depelacment juste a gouche et droit</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> commence la partie La classe Missile</t>
+  </si>
+  <si>
+    <t>j'ai commencé la La classe Missile</t>
   </si>
 </sst>
 </file>
@@ -908,7 +941,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="99">
+  <cellXfs count="100">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1152,16 +1185,6 @@
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1182,6 +1205,19 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -1569,7 +1605,7 @@
                   <a14:compatExt spid="_x0000_s46081"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D09E1A6C-B10D-46E2-BA28-F032825CEFAB}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000001B40000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1632,7 +1668,7 @@
                   <a14:compatExt spid="_x0000_s45057"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{82F62593-241C-4DD9-9D8B-1C4F4FD87C82}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000001B00000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1902,7 +1938,7 @@
   </sheetPr>
   <dimension ref="A1:M73"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -2119,10 +2155,10 @@
     </row>
     <row r="19" spans="1:13" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="79"/>
-      <c r="B19" s="88" t="s">
+      <c r="B19" s="95" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="89"/>
+      <c r="C19" s="96"/>
       <c r="D19" s="60"/>
       <c r="E19" s="60"/>
       <c r="F19" s="60"/>
@@ -3067,7 +3103,7 @@
     </row>
     <row r="3" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="19"/>
-      <c r="B3" s="90" t="s">
+      <c r="B3" s="97" t="s">
         <v>21</v>
       </c>
       <c r="C3" s="16">
@@ -3076,7 +3112,7 @@
     </row>
     <row r="4" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="19"/>
-      <c r="B4" s="91"/>
+      <c r="B4" s="98"/>
       <c r="C4" s="22">
         <v>0</v>
       </c>
@@ -3879,8 +3915,8 @@
   <sheetPr codeName="Feuil5"/>
   <dimension ref="A1:I281"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C269" sqref="C269"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -3919,7 +3955,7 @@
     <row r="3" spans="1:4" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
       <c r="B3" s="4"/>
-      <c r="C3" s="95">
+      <c r="C3" s="91">
         <v>45309</v>
       </c>
       <c r="D3" s="9"/>
@@ -3931,7 +3967,7 @@
       <c r="B4" s="2">
         <v>1</v>
       </c>
-      <c r="C4" s="96" t="s">
+      <c r="C4" s="92" t="s">
         <v>41</v>
       </c>
       <c r="D4" s="10"/>
@@ -3943,10 +3979,10 @@
       <c r="B5" s="2">
         <v>1</v>
       </c>
-      <c r="C5" s="96" t="s">
+      <c r="C5" s="92" t="s">
         <v>42</v>
       </c>
-      <c r="D5" s="98" t="s">
+      <c r="D5" s="94" t="s">
         <v>43</v>
       </c>
     </row>
@@ -3957,21 +3993,27 @@
       <c r="B6" s="2">
         <v>1</v>
       </c>
-      <c r="C6" s="96" t="s">
+      <c r="C6" s="92" t="s">
         <v>40</v>
       </c>
-      <c r="D6" s="96"/>
+      <c r="D6" s="92"/>
     </row>
     <row r="7" spans="1:4" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="10"/>
+      <c r="A7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="2">
+        <v>1</v>
+      </c>
+      <c r="C7" s="92" t="s">
+        <v>66</v>
+      </c>
       <c r="D7" s="10"/>
     </row>
     <row r="8" spans="1:4" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="2"/>
-      <c r="C8" s="96" t="s">
+      <c r="C8" s="92" t="s">
         <v>44</v>
       </c>
       <c r="D8" s="10"/>
@@ -3983,7 +4025,7 @@
       <c r="B9" s="2">
         <v>1</v>
       </c>
-      <c r="C9" s="96" t="s">
+      <c r="C9" s="92" t="s">
         <v>45</v>
       </c>
       <c r="D9" s="10"/>
@@ -4012,9 +4054,9 @@
       </c>
       <c r="B13" s="12">
         <f>SUM(B3:B12)</f>
-        <v>4</v>
-      </c>
-      <c r="C13" s="92" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="88" t="s">
         <v>34</v>
       </c>
       <c r="D13" s="13"/>
@@ -4049,24 +4091,36 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="5"/>
       <c r="B17" s="4"/>
-      <c r="C17" s="97" t="s">
+      <c r="C17" s="99">
+        <v>45316</v>
+      </c>
+      <c r="D17" s="9"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" s="2">
+        <v>2</v>
+      </c>
+      <c r="C18" s="93" t="s">
         <v>46</v>
       </c>
-      <c r="D17" s="9"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="10"/>
       <c r="D18" s="10"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="10"/>
+      <c r="A19" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B19" s="2">
+        <v>2</v>
+      </c>
+      <c r="C19" s="92" t="s">
+        <v>69</v>
+      </c>
       <c r="D19" s="10"/>
       <c r="E19" s="20"/>
       <c r="F19" s="20"/>
@@ -4077,7 +4131,9 @@
     <row r="20" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="2"/>
-      <c r="C20" s="10"/>
+      <c r="C20" s="92" t="s">
+        <v>70</v>
+      </c>
       <c r="D20" s="10"/>
       <c r="E20" s="20"/>
       <c r="F20" s="32"/>
@@ -4157,9 +4213,9 @@
       </c>
       <c r="B27" s="12">
         <f>SUM(B17:B26)</f>
-        <v>0</v>
-      </c>
-      <c r="C27" s="92" t="s">
+        <v>4</v>
+      </c>
+      <c r="C27" s="88" t="s">
         <v>34</v>
       </c>
       <c r="D27" s="13"/>
@@ -4214,11 +4270,11 @@
       <c r="H30" s="40"/>
       <c r="I30" s="20"/>
     </row>
-    <row r="31" spans="1:9" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="5"/>
       <c r="B31" s="4"/>
-      <c r="C31" s="97" t="s">
-        <v>37</v>
+      <c r="C31" s="99">
+        <v>45323</v>
       </c>
       <c r="D31" s="9"/>
       <c r="E31" s="20"/>
@@ -4230,7 +4286,9 @@
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="2"/>
-      <c r="C32" s="10"/>
+      <c r="C32" s="93" t="s">
+        <v>37</v>
+      </c>
       <c r="D32" s="10"/>
       <c r="E32" s="20"/>
       <c r="F32" s="20"/>
@@ -4239,9 +4297,15 @@
       <c r="I32" s="20"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="1"/>
-      <c r="B33" s="2"/>
-      <c r="C33" s="10"/>
+      <c r="A33" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B33" s="2">
+        <v>2</v>
+      </c>
+      <c r="C33" s="92" t="s">
+        <v>75</v>
+      </c>
       <c r="D33" s="10"/>
       <c r="E33" s="20"/>
       <c r="F33" s="20"/>
@@ -4250,9 +4314,15 @@
       <c r="I33" s="20"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="1"/>
-      <c r="B34" s="2"/>
-      <c r="C34" s="10"/>
+      <c r="A34" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B34" s="2">
+        <v>1</v>
+      </c>
+      <c r="C34" s="92" t="s">
+        <v>76</v>
+      </c>
       <c r="D34" s="10"/>
       <c r="E34" s="20"/>
       <c r="F34" s="20"/>
@@ -4302,9 +4372,9 @@
       </c>
       <c r="B41" s="12">
         <f>SUM(B31:B40)</f>
-        <v>0</v>
-      </c>
-      <c r="C41" s="92" t="s">
+        <v>3</v>
+      </c>
+      <c r="C41" s="88" t="s">
         <v>34</v>
       </c>
       <c r="D41" s="13"/>
@@ -4342,7 +4412,7 @@
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="5"/>
       <c r="B45" s="4"/>
-      <c r="C45" s="97" t="s">
+      <c r="C45" s="93" t="s">
         <v>47</v>
       </c>
       <c r="D45" s="9"/>
@@ -4409,7 +4479,7 @@
         <f>SUM(B45:B54)</f>
         <v>0</v>
       </c>
-      <c r="C55" s="92" t="s">
+      <c r="C55" s="88" t="s">
         <v>34</v>
       </c>
       <c r="D55" s="13"/>
@@ -4447,7 +4517,7 @@
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="5"/>
       <c r="B59" s="4"/>
-      <c r="C59" s="97" t="s">
+      <c r="C59" s="93" t="s">
         <v>48</v>
       </c>
       <c r="D59" s="9"/>
@@ -4514,7 +4584,7 @@
         <f>SUM(B59:B68)</f>
         <v>0</v>
       </c>
-      <c r="C69" s="92" t="s">
+      <c r="C69" s="88" t="s">
         <v>34</v>
       </c>
       <c r="D69" s="13"/>
@@ -4552,7 +4622,7 @@
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="5"/>
       <c r="B73" s="4"/>
-      <c r="C73" s="97" t="s">
+      <c r="C73" s="93" t="s">
         <v>38</v>
       </c>
       <c r="D73" s="9"/>
@@ -4619,7 +4689,7 @@
         <f>SUM(B73:B82)</f>
         <v>0</v>
       </c>
-      <c r="C83" s="92" t="s">
+      <c r="C83" s="88" t="s">
         <v>34</v>
       </c>
       <c r="D83" s="13"/>
@@ -4657,7 +4727,7 @@
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="5"/>
       <c r="B87" s="4"/>
-      <c r="C87" s="97" t="s">
+      <c r="C87" s="93" t="s">
         <v>49</v>
       </c>
       <c r="D87" s="9"/>
@@ -4724,7 +4794,7 @@
         <f>SUM(B87:B96)</f>
         <v>0</v>
       </c>
-      <c r="C97" s="92" t="s">
+      <c r="C97" s="88" t="s">
         <v>34</v>
       </c>
       <c r="D97" s="13"/>
@@ -4762,7 +4832,7 @@
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="5"/>
       <c r="B101" s="4"/>
-      <c r="C101" s="97" t="s">
+      <c r="C101" s="93" t="s">
         <v>50</v>
       </c>
       <c r="D101" s="9"/>
@@ -4829,7 +4899,7 @@
         <f>SUM(B101:B110)</f>
         <v>0</v>
       </c>
-      <c r="C111" s="92" t="s">
+      <c r="C111" s="88" t="s">
         <v>34</v>
       </c>
       <c r="D111" s="13"/>
@@ -4867,7 +4937,7 @@
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" s="5"/>
       <c r="B115" s="4"/>
-      <c r="C115" s="97" t="s">
+      <c r="C115" s="93" t="s">
         <v>39</v>
       </c>
       <c r="D115" s="9"/>
@@ -4934,7 +5004,7 @@
         <f>SUM(B115:B124)</f>
         <v>0</v>
       </c>
-      <c r="C125" s="92" t="s">
+      <c r="C125" s="88" t="s">
         <v>34</v>
       </c>
       <c r="D125" s="13"/>
@@ -4972,7 +5042,7 @@
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" s="5"/>
       <c r="B129" s="4"/>
-      <c r="C129" s="97" t="s">
+      <c r="C129" s="93" t="s">
         <v>51</v>
       </c>
       <c r="D129" s="9"/>
@@ -5039,7 +5109,7 @@
         <f>SUM(B129:B138)</f>
         <v>0</v>
       </c>
-      <c r="C139" s="92" t="s">
+      <c r="C139" s="88" t="s">
         <v>34</v>
       </c>
       <c r="D139" s="13"/>
@@ -5077,7 +5147,7 @@
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" s="5"/>
       <c r="B143" s="4"/>
-      <c r="C143" s="97" t="s">
+      <c r="C143" s="93" t="s">
         <v>52</v>
       </c>
       <c r="D143" s="9"/>
@@ -5144,7 +5214,7 @@
         <f>SUM(B143:B152)</f>
         <v>0</v>
       </c>
-      <c r="C153" s="92" t="s">
+      <c r="C153" s="88" t="s">
         <v>34</v>
       </c>
       <c r="D153" s="13"/>
@@ -5182,7 +5252,7 @@
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" s="5"/>
       <c r="B157" s="4"/>
-      <c r="C157" s="97" t="s">
+      <c r="C157" s="93" t="s">
         <v>53</v>
       </c>
       <c r="D157" s="9"/>
@@ -5249,7 +5319,7 @@
         <f>SUM(B157:B166)</f>
         <v>0</v>
       </c>
-      <c r="C167" s="92" t="s">
+      <c r="C167" s="88" t="s">
         <v>34</v>
       </c>
       <c r="D167" s="13"/>
@@ -5287,7 +5357,7 @@
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A171" s="5"/>
       <c r="B171" s="4"/>
-      <c r="C171" s="97" t="s">
+      <c r="C171" s="93" t="s">
         <v>54</v>
       </c>
       <c r="D171" s="9"/>
@@ -5354,7 +5424,7 @@
         <f>SUM(B171:B180)</f>
         <v>0</v>
       </c>
-      <c r="C181" s="92" t="s">
+      <c r="C181" s="88" t="s">
         <v>34</v>
       </c>
       <c r="D181" s="13"/>
@@ -5392,7 +5462,7 @@
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A185" s="5"/>
       <c r="B185" s="4"/>
-      <c r="C185" s="97" t="s">
+      <c r="C185" s="93" t="s">
         <v>55</v>
       </c>
       <c r="D185" s="9"/>
@@ -5459,7 +5529,7 @@
         <f>SUM(B185:B194)</f>
         <v>0</v>
       </c>
-      <c r="C195" s="92" t="s">
+      <c r="C195" s="88" t="s">
         <v>34</v>
       </c>
       <c r="D195" s="13"/>
@@ -5497,7 +5567,7 @@
     <row r="199" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A199" s="5"/>
       <c r="B199" s="4"/>
-      <c r="C199" s="97" t="s">
+      <c r="C199" s="93" t="s">
         <v>56</v>
       </c>
       <c r="D199" s="9"/>
@@ -5564,7 +5634,7 @@
         <f>SUM(B199:B208)</f>
         <v>0</v>
       </c>
-      <c r="C209" s="92" t="s">
+      <c r="C209" s="88" t="s">
         <v>34</v>
       </c>
       <c r="D209" s="13"/>
@@ -5602,7 +5672,7 @@
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A213" s="5"/>
       <c r="B213" s="4"/>
-      <c r="C213" s="97" t="s">
+      <c r="C213" s="93" t="s">
         <v>57</v>
       </c>
       <c r="D213" s="9"/>
@@ -5669,7 +5739,7 @@
         <f>SUM(B213:B222)</f>
         <v>0</v>
       </c>
-      <c r="C223" s="92" t="s">
+      <c r="C223" s="88" t="s">
         <v>34</v>
       </c>
       <c r="D223" s="13"/>
@@ -5707,7 +5777,7 @@
     <row r="227" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A227" s="5"/>
       <c r="B227" s="4"/>
-      <c r="C227" s="97" t="s">
+      <c r="C227" s="93" t="s">
         <v>58</v>
       </c>
       <c r="D227" s="9"/>
@@ -5774,7 +5844,7 @@
         <f>SUM(B227:B236)</f>
         <v>0</v>
       </c>
-      <c r="C237" s="92" t="s">
+      <c r="C237" s="88" t="s">
         <v>34</v>
       </c>
       <c r="D237" s="13"/>
@@ -5812,7 +5882,7 @@
     <row r="241" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A241" s="5"/>
       <c r="B241" s="4"/>
-      <c r="C241" s="97" t="s">
+      <c r="C241" s="93" t="s">
         <v>59</v>
       </c>
       <c r="D241" s="9"/>
@@ -5844,7 +5914,7 @@
     <row r="246" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A246" s="1"/>
       <c r="B246" s="2"/>
-      <c r="C246" s="96" t="s">
+      <c r="C246" s="92" t="s">
         <v>60</v>
       </c>
       <c r="D246" s="10"/>
@@ -5881,7 +5951,7 @@
         <f>SUM(B241:B250)</f>
         <v>0</v>
       </c>
-      <c r="C251" s="92" t="s">
+      <c r="C251" s="88" t="s">
         <v>34</v>
       </c>
       <c r="D251" s="13"/>
@@ -5919,7 +5989,7 @@
     <row r="255" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A255" s="5"/>
       <c r="B255" s="4"/>
-      <c r="C255" s="97" t="s">
+      <c r="C255" s="93" t="s">
         <v>61</v>
       </c>
       <c r="D255" s="9"/>
@@ -5986,7 +6056,7 @@
         <f>SUM(B255:B264)</f>
         <v>0</v>
       </c>
-      <c r="C265" s="92" t="s">
+      <c r="C265" s="88" t="s">
         <v>34</v>
       </c>
       <c r="D265" s="13"/>
@@ -6024,7 +6094,7 @@
     <row r="269" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A269" s="5"/>
       <c r="B269" s="4"/>
-      <c r="C269" s="97" t="s">
+      <c r="C269" s="93" t="s">
         <v>62</v>
       </c>
       <c r="D269" s="9"/>
@@ -6091,7 +6161,7 @@
         <f>SUM(B269:B278)</f>
         <v>0</v>
       </c>
-      <c r="C279" s="92" t="s">
+      <c r="C279" s="88" t="s">
         <v>34</v>
       </c>
       <c r="D279" s="13"/>
@@ -6103,7 +6173,7 @@
       <c r="D280" s="14"/>
     </row>
     <row r="281" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A281" s="93" t="s">
+      <c r="A281" s="89" t="s">
         <v>35</v>
       </c>
     </row>
@@ -6164,8 +6234,8 @@
   <sheetPr codeName="Feuil9"/>
   <dimension ref="A1:I381"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -6213,7 +6283,7 @@
       <c r="B3" s="4">
         <v>1</v>
       </c>
-      <c r="C3" s="97" t="s">
+      <c r="C3" s="93" t="s">
         <v>63</v>
       </c>
       <c r="D3" s="9"/>
@@ -6225,7 +6295,7 @@
       <c r="B4" s="2">
         <v>1</v>
       </c>
-      <c r="C4" s="96" t="s">
+      <c r="C4" s="92" t="s">
         <v>64</v>
       </c>
       <c r="D4" s="10"/>
@@ -6237,33 +6307,36 @@
       <c r="B5" s="2">
         <v>1</v>
       </c>
-      <c r="C5" s="96" t="s">
-        <v>65</v>
+      <c r="C5" s="53" t="s">
+        <v>67</v>
       </c>
       <c r="D5" s="10"/>
     </row>
-    <row r="6" spans="1:4" s="53" customFormat="1" ht="27" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B6" s="2">
         <v>1</v>
       </c>
-      <c r="C6" s="96" t="s">
-        <v>66</v>
+      <c r="C6" s="92" t="s">
+        <v>65</v>
       </c>
       <c r="D6" s="10"/>
     </row>
-    <row r="7" spans="1:4" s="53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" s="53" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="10"/>
+      <c r="B7" s="2">
+        <v>1</v>
+      </c>
+      <c r="C7" s="92" t="s">
+        <v>68</v>
+      </c>
       <c r="D7" s="10"/>
     </row>
     <row r="8" spans="1:4" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="2"/>
-      <c r="C8" s="10"/>
       <c r="D8" s="10"/>
     </row>
     <row r="9" spans="1:4" s="53" customFormat="1" x14ac:dyDescent="0.25">
@@ -6326,9 +6399,9 @@
       </c>
       <c r="B18" s="48">
         <f>SUM(B3:B17)</f>
-        <v>4</v>
-      </c>
-      <c r="C18" s="94" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="90" t="s">
         <v>34</v>
       </c>
       <c r="D18" s="49"/>
@@ -6375,15 +6448,27 @@
       <c r="D22" s="9"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="1"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="10"/>
+      <c r="A23" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B23" s="2">
+        <v>2</v>
+      </c>
+      <c r="C23" s="92" t="s">
+        <v>71</v>
+      </c>
       <c r="D23" s="10"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="1"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="10"/>
+      <c r="A24" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B24" s="2">
+        <v>1</v>
+      </c>
+      <c r="C24" s="92" t="s">
+        <v>72</v>
+      </c>
       <c r="D24" s="10"/>
       <c r="E24" s="20"/>
       <c r="F24" s="20"/>
@@ -6393,8 +6478,12 @@
     </row>
     <row r="25" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
-      <c r="B25" s="2"/>
-      <c r="C25" s="10"/>
+      <c r="B25" s="2">
+        <v>1</v>
+      </c>
+      <c r="C25" s="92" t="s">
+        <v>73</v>
+      </c>
       <c r="D25" s="10"/>
       <c r="E25" s="20"/>
       <c r="F25" s="32"/>
@@ -6529,9 +6618,9 @@
       </c>
       <c r="B37" s="48">
         <f>SUM(B22:B36)</f>
-        <v>0</v>
-      </c>
-      <c r="C37" s="94" t="s">
+        <v>4</v>
+      </c>
+      <c r="C37" s="90" t="s">
         <v>34</v>
       </c>
       <c r="D37" s="49"/>
@@ -6593,15 +6682,25 @@
       <c r="D41" s="9"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="1"/>
-      <c r="B42" s="2"/>
-      <c r="C42" s="10"/>
+      <c r="A42" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B42" s="2">
+        <v>2</v>
+      </c>
+      <c r="C42" s="92" t="s">
+        <v>74</v>
+      </c>
       <c r="D42" s="10"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
-      <c r="B43" s="2"/>
-      <c r="C43" s="10"/>
+      <c r="B43" s="2">
+        <v>1</v>
+      </c>
+      <c r="C43" s="92" t="s">
+        <v>77</v>
+      </c>
       <c r="D43" s="10"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
@@ -6682,9 +6781,9 @@
       </c>
       <c r="B56" s="48">
         <f>SUM(B41:B55)</f>
-        <v>0</v>
-      </c>
-      <c r="C56" s="94" t="s">
+        <v>3</v>
+      </c>
+      <c r="C56" s="90" t="s">
         <v>34</v>
       </c>
       <c r="D56" s="49"/>
@@ -6822,7 +6921,7 @@
         <f>SUM(B60:B74)</f>
         <v>0</v>
       </c>
-      <c r="C75" s="94" t="s">
+      <c r="C75" s="90" t="s">
         <v>34</v>
       </c>
       <c r="D75" s="49"/>
@@ -6960,7 +7059,7 @@
         <f>SUM(B79:B93)</f>
         <v>0</v>
       </c>
-      <c r="C94" s="94" t="s">
+      <c r="C94" s="90" t="s">
         <v>34</v>
       </c>
       <c r="D94" s="49"/>
@@ -7098,7 +7197,7 @@
         <f>SUM(B98:B112)</f>
         <v>0</v>
       </c>
-      <c r="C113" s="94" t="s">
+      <c r="C113" s="90" t="s">
         <v>34</v>
       </c>
       <c r="D113" s="49"/>
@@ -7236,7 +7335,7 @@
         <f>SUM(B117:B131)</f>
         <v>0</v>
       </c>
-      <c r="C132" s="94" t="s">
+      <c r="C132" s="90" t="s">
         <v>34</v>
       </c>
       <c r="D132" s="49"/>
@@ -7374,7 +7473,7 @@
         <f>SUM(B136:B150)</f>
         <v>0</v>
       </c>
-      <c r="C151" s="94" t="s">
+      <c r="C151" s="90" t="s">
         <v>34</v>
       </c>
       <c r="D151" s="49"/>
@@ -7512,7 +7611,7 @@
         <f>SUM(B155:B169)</f>
         <v>0</v>
       </c>
-      <c r="C170" s="94" t="s">
+      <c r="C170" s="90" t="s">
         <v>34</v>
       </c>
       <c r="D170" s="49"/>
@@ -7650,7 +7749,7 @@
         <f>SUM(B174:B188)</f>
         <v>0</v>
       </c>
-      <c r="C189" s="94" t="s">
+      <c r="C189" s="90" t="s">
         <v>34</v>
       </c>
       <c r="D189" s="49"/>
@@ -7788,7 +7887,7 @@
         <f>SUM(B193:B207)</f>
         <v>0</v>
       </c>
-      <c r="C208" s="94" t="s">
+      <c r="C208" s="90" t="s">
         <v>34</v>
       </c>
       <c r="D208" s="49"/>
@@ -7926,7 +8025,7 @@
         <f>SUM(B212:B226)</f>
         <v>0</v>
       </c>
-      <c r="C227" s="94" t="s">
+      <c r="C227" s="90" t="s">
         <v>34</v>
       </c>
       <c r="D227" s="49"/>
@@ -8064,7 +8163,7 @@
         <f>SUM(B231:B245)</f>
         <v>0</v>
       </c>
-      <c r="C246" s="94" t="s">
+      <c r="C246" s="90" t="s">
         <v>34</v>
       </c>
       <c r="D246" s="49"/>
@@ -8202,7 +8301,7 @@
         <f>SUM(B250:B264)</f>
         <v>0</v>
       </c>
-      <c r="C265" s="94" t="s">
+      <c r="C265" s="90" t="s">
         <v>34</v>
       </c>
       <c r="D265" s="49"/>
@@ -8340,7 +8439,7 @@
         <f>SUM(B269:B283)</f>
         <v>0</v>
       </c>
-      <c r="C284" s="94" t="s">
+      <c r="C284" s="90" t="s">
         <v>34</v>
       </c>
       <c r="D284" s="49"/>
@@ -8478,7 +8577,7 @@
         <f>SUM(B288:B302)</f>
         <v>0</v>
       </c>
-      <c r="C303" s="94" t="s">
+      <c r="C303" s="90" t="s">
         <v>34</v>
       </c>
       <c r="D303" s="49"/>
@@ -8616,7 +8715,7 @@
         <f>SUM(B307:B321)</f>
         <v>0</v>
       </c>
-      <c r="C322" s="94" t="s">
+      <c r="C322" s="90" t="s">
         <v>34</v>
       </c>
       <c r="D322" s="49"/>
@@ -8754,7 +8853,7 @@
         <f>SUM(B326:B340)</f>
         <v>0</v>
       </c>
-      <c r="C341" s="94" t="s">
+      <c r="C341" s="90" t="s">
         <v>34</v>
       </c>
       <c r="D341" s="49"/>
@@ -8892,7 +8991,7 @@
         <f>SUM(B345:B359)</f>
         <v>0</v>
       </c>
-      <c r="C360" s="94" t="s">
+      <c r="C360" s="90" t="s">
         <v>34</v>
       </c>
       <c r="D360" s="49"/>
@@ -9030,7 +9129,7 @@
         <f>SUM(B364:B378)</f>
         <v>0</v>
       </c>
-      <c r="C379" s="94" t="s">
+      <c r="C379" s="90" t="s">
         <v>34</v>
       </c>
       <c r="D379" s="49"/>
@@ -9042,7 +9141,7 @@
       <c r="D380" s="50"/>
     </row>
     <row r="381" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A381" s="93" t="s">
+      <c r="A381" s="89" t="s">
         <v>35</v>
       </c>
     </row>

</xml_diff>

<commit_message>
j'ai commencé a coder pour tirer
</commit_message>
<xml_diff>
--- a/Docs/planification-Projet-Hanieh Mohajerani.xlsx
+++ b/Docs/planification-Projet-Hanieh Mohajerani.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Cours-Semestre\Semestres\Semestre 1-2\Projet-Module-C#\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDC79EB8-B8AE-43B0-8A6C-84A863302498}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBB34F13-55C5-4881-BA2D-A924F4D5FCAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Donnees" sheetId="7" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="83">
   <si>
     <t>Module :</t>
   </si>
@@ -211,9 +211,6 @@
     <t>3)Création du vaisseau du joueur</t>
   </si>
   <si>
-    <t>5)La classe Missile</t>
-  </si>
-  <si>
     <t>6)Tir du joueur</t>
   </si>
   <si>
@@ -301,7 +298,25 @@
     <t xml:space="preserve"> commence la partie La classe Missile</t>
   </si>
   <si>
-    <t>j'ai commencé la La classe Missile</t>
+    <t>j'ai commencé la La classe Missile,et j'ai crée la  classe Missile pour permettre au joueur de tirer</t>
+  </si>
+  <si>
+    <t>j'ai encor travailé sur la position de objet pour aller gouch et droit</t>
+  </si>
+  <si>
+    <t>5)La classe Missile                                                                                                       08.02.2024</t>
+  </si>
+  <si>
+    <t>creer La classe Missile</t>
+  </si>
+  <si>
+    <t>j'ai creé La classe Missile  qui hérite de la classe GameObject</t>
+  </si>
+  <si>
+    <t xml:space="preserve">corrige le cod pour tirer </t>
+  </si>
+  <si>
+    <t>j'ai crée les méthodes abstraites de la classe GameObject et j'ai commencé codé pour tirer</t>
   </si>
 </sst>
 </file>
@@ -311,7 +326,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Century Gothic"/>
@@ -420,6 +435,12 @@
       <name val="Century Gothic"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF404040"/>
+      <name val="Lato"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="14">
@@ -941,7 +962,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="100">
+  <cellXfs count="101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1207,6 +1228,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1217,9 +1241,7 @@
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -1938,7 +1960,7 @@
   </sheetPr>
   <dimension ref="A1:M73"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -2155,10 +2177,10 @@
     </row>
     <row r="19" spans="1:13" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="79"/>
-      <c r="B19" s="95" t="s">
+      <c r="B19" s="96" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="96"/>
+      <c r="C19" s="97"/>
       <c r="D19" s="60"/>
       <c r="E19" s="60"/>
       <c r="F19" s="60"/>
@@ -3103,7 +3125,7 @@
     </row>
     <row r="3" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="19"/>
-      <c r="B3" s="97" t="s">
+      <c r="B3" s="98" t="s">
         <v>21</v>
       </c>
       <c r="C3" s="16">
@@ -3112,7 +3134,7 @@
     </row>
     <row r="4" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="19"/>
-      <c r="B4" s="98"/>
+      <c r="B4" s="99"/>
       <c r="C4" s="22">
         <v>0</v>
       </c>
@@ -3915,8 +3937,8 @@
   <sheetPr codeName="Feuil5"/>
   <dimension ref="A1:I281"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -4006,7 +4028,7 @@
         <v>1</v>
       </c>
       <c r="C7" s="92" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D7" s="10"/>
     </row>
@@ -4094,7 +4116,7 @@
     <row r="17" spans="1:9" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="5"/>
       <c r="B17" s="4"/>
-      <c r="C17" s="99">
+      <c r="C17" s="95">
         <v>45316</v>
       </c>
       <c r="D17" s="9"/>
@@ -4119,7 +4141,7 @@
         <v>2</v>
       </c>
       <c r="C19" s="92" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D19" s="10"/>
       <c r="E19" s="20"/>
@@ -4132,7 +4154,7 @@
       <c r="A20" s="1"/>
       <c r="B20" s="2"/>
       <c r="C20" s="92" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D20" s="10"/>
       <c r="E20" s="20"/>
@@ -4273,7 +4295,7 @@
     <row r="31" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="5"/>
       <c r="B31" s="4"/>
-      <c r="C31" s="99">
+      <c r="C31" s="95">
         <v>45323</v>
       </c>
       <c r="D31" s="9"/>
@@ -4304,7 +4326,7 @@
         <v>2</v>
       </c>
       <c r="C33" s="92" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D33" s="10"/>
       <c r="E33" s="20"/>
@@ -4321,7 +4343,7 @@
         <v>1</v>
       </c>
       <c r="C34" s="92" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D34" s="10"/>
       <c r="E34" s="20"/>
@@ -4413,20 +4435,28 @@
       <c r="A45" s="5"/>
       <c r="B45" s="4"/>
       <c r="C45" s="93" t="s">
-        <v>47</v>
+        <v>78</v>
       </c>
       <c r="D45" s="9"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
-      <c r="B46" s="2"/>
-      <c r="C46" s="10"/>
+      <c r="B46" s="2">
+        <v>2</v>
+      </c>
+      <c r="C46" s="92" t="s">
+        <v>79</v>
+      </c>
       <c r="D46" s="10"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
-      <c r="B47" s="2"/>
-      <c r="C47" s="10"/>
+      <c r="B47" s="2">
+        <v>2</v>
+      </c>
+      <c r="C47" s="92" t="s">
+        <v>81</v>
+      </c>
       <c r="D47" s="10"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
@@ -4477,7 +4507,7 @@
       </c>
       <c r="B55" s="12">
         <f>SUM(B45:B54)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C55" s="88" t="s">
         <v>34</v>
@@ -4518,7 +4548,7 @@
       <c r="A59" s="5"/>
       <c r="B59" s="4"/>
       <c r="C59" s="93" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D59" s="9"/>
     </row>
@@ -4728,7 +4758,7 @@
       <c r="A87" s="5"/>
       <c r="B87" s="4"/>
       <c r="C87" s="93" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D87" s="9"/>
     </row>
@@ -4833,7 +4863,7 @@
       <c r="A101" s="5"/>
       <c r="B101" s="4"/>
       <c r="C101" s="93" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D101" s="9"/>
     </row>
@@ -5043,7 +5073,7 @@
       <c r="A129" s="5"/>
       <c r="B129" s="4"/>
       <c r="C129" s="93" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D129" s="9"/>
     </row>
@@ -5148,7 +5178,7 @@
       <c r="A143" s="5"/>
       <c r="B143" s="4"/>
       <c r="C143" s="93" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D143" s="9"/>
     </row>
@@ -5253,7 +5283,7 @@
       <c r="A157" s="5"/>
       <c r="B157" s="4"/>
       <c r="C157" s="93" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D157" s="9"/>
     </row>
@@ -5358,7 +5388,7 @@
       <c r="A171" s="5"/>
       <c r="B171" s="4"/>
       <c r="C171" s="93" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D171" s="9"/>
     </row>
@@ -5463,7 +5493,7 @@
       <c r="A185" s="5"/>
       <c r="B185" s="4"/>
       <c r="C185" s="93" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D185" s="9"/>
     </row>
@@ -5568,7 +5598,7 @@
       <c r="A199" s="5"/>
       <c r="B199" s="4"/>
       <c r="C199" s="93" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D199" s="9"/>
     </row>
@@ -5673,7 +5703,7 @@
       <c r="A213" s="5"/>
       <c r="B213" s="4"/>
       <c r="C213" s="93" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D213" s="9"/>
     </row>
@@ -5778,7 +5808,7 @@
       <c r="A227" s="5"/>
       <c r="B227" s="4"/>
       <c r="C227" s="93" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D227" s="9"/>
     </row>
@@ -5883,7 +5913,7 @@
       <c r="A241" s="5"/>
       <c r="B241" s="4"/>
       <c r="C241" s="93" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D241" s="9"/>
     </row>
@@ -5915,7 +5945,7 @@
       <c r="A246" s="1"/>
       <c r="B246" s="2"/>
       <c r="C246" s="92" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D246" s="10"/>
     </row>
@@ -5990,7 +6020,7 @@
       <c r="A255" s="5"/>
       <c r="B255" s="4"/>
       <c r="C255" s="93" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D255" s="9"/>
     </row>
@@ -6095,7 +6125,7 @@
       <c r="A269" s="5"/>
       <c r="B269" s="4"/>
       <c r="C269" s="93" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D269" s="9"/>
     </row>
@@ -6234,8 +6264,8 @@
   <sheetPr codeName="Feuil9"/>
   <dimension ref="A1:I381"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="C63" sqref="C63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -6284,7 +6314,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="93" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D3" s="9"/>
     </row>
@@ -6296,7 +6326,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="92" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D4" s="10"/>
     </row>
@@ -6308,7 +6338,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="53" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D5" s="10"/>
     </row>
@@ -6320,7 +6350,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="92" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D6" s="10"/>
     </row>
@@ -6330,7 +6360,7 @@
         <v>1</v>
       </c>
       <c r="C7" s="92" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D7" s="10"/>
     </row>
@@ -6455,7 +6485,7 @@
         <v>2</v>
       </c>
       <c r="C23" s="92" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D23" s="10"/>
     </row>
@@ -6467,7 +6497,7 @@
         <v>1</v>
       </c>
       <c r="C24" s="92" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D24" s="10"/>
       <c r="E24" s="20"/>
@@ -6482,7 +6512,7 @@
         <v>1</v>
       </c>
       <c r="C25" s="92" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D25" s="10"/>
       <c r="E25" s="20"/>
@@ -6689,17 +6719,17 @@
         <v>2</v>
       </c>
       <c r="C42" s="92" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D42" s="10"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" ht="27" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="2">
         <v>1</v>
       </c>
       <c r="C43" s="92" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D43" s="10"/>
     </row>
@@ -6830,21 +6860,37 @@
       <c r="D60" s="9"/>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="1"/>
-      <c r="B61" s="2"/>
-      <c r="C61" s="10"/>
+      <c r="A61" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B61" s="2">
+        <v>2</v>
+      </c>
+      <c r="C61" s="92" t="s">
+        <v>77</v>
+      </c>
       <c r="D61" s="10"/>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="1"/>
-      <c r="B62" s="2"/>
-      <c r="C62" s="10"/>
+      <c r="A62" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B62" s="2">
+        <v>1</v>
+      </c>
+      <c r="C62" s="92" t="s">
+        <v>80</v>
+      </c>
       <c r="D62" s="10"/>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="A63" s="1"/>
-      <c r="B63" s="2"/>
-      <c r="C63" s="10"/>
+      <c r="B63" s="2">
+        <v>1</v>
+      </c>
+      <c r="C63" s="100" t="s">
+        <v>82</v>
+      </c>
       <c r="D63" s="10"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -6919,7 +6965,7 @@
       </c>
       <c r="B75" s="48">
         <f>SUM(B60:B74)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C75" s="90" t="s">
         <v>34</v>

</xml_diff>

<commit_message>
j'ai cree 1 nouveu projet et j'ai ajouté l'enemie que tire depuis haut mais je doit corriger depelecment de missile j'ai ajouté les murs et les position de objet en bas est juste et il tire et bouge la même temps
</commit_message>
<xml_diff>
--- a/Docs/planification-Projet-Hanieh Mohajerani.xlsx
+++ b/Docs/planification-Projet-Hanieh Mohajerani.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26731"/>
   <workbookPr updateLinks="never" codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Cours-Semestre\Semestres\Semestre 1-2\Projet-Module-C#\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C2C9BA9-0C68-490E-B26C-78C006FB7C88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CA51BE5-A3AB-4AF6-8272-9958525B319F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="96">
   <si>
     <t>Module :</t>
   </si>
@@ -344,6 +344,18 @@
   </si>
   <si>
     <t>lênemie va a gouche et droit mais il tire pas juste</t>
+  </si>
+  <si>
+    <t>j'ai creé les murs</t>
+  </si>
+  <si>
+    <t>j'ai modifier l'objet en bas que tire juste</t>
+  </si>
+  <si>
+    <t>j'ai testé avec des chiffre differents</t>
+  </si>
+  <si>
+    <t>j'ai corrigé les missiles car avant les missiles d'enemie a marché pas juste mais ce n'a pas encore fini</t>
   </si>
 </sst>
 </file>
@@ -1257,6 +1269,14 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1267,14 +1287,6 @@
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -2210,10 +2222,10 @@
     </row>
     <row r="19" spans="1:7" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="78"/>
-      <c r="B19" s="95" t="s">
+      <c r="B19" s="97" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="96"/>
+      <c r="C19" s="98"/>
       <c r="D19" s="59"/>
       <c r="E19" s="59"/>
       <c r="F19" s="59"/>
@@ -2620,27 +2632,27 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="15364" r:id="rId5" name="btnCreatePlanning">
+        <control shapeId="15365" r:id="rId5" name="btnCreateWorkSheet">
           <controlPr defaultSize="0" autoLine="0" r:id="rId6">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>5</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
+                <xdr:row>8</xdr:row>
+                <xdr:rowOff>190500</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>6</xdr:col>
-                <xdr:colOff>95250</xdr:colOff>
-                <xdr:row>7</xdr:row>
-                <xdr:rowOff>47625</xdr:rowOff>
+                <xdr:colOff>114300</xdr:colOff>
+                <xdr:row>10</xdr:row>
+                <xdr:rowOff>152400</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="15364" r:id="rId5" name="btnCreatePlanning"/>
+        <control shapeId="15365" r:id="rId5" name="btnCreateWorkSheet"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -2670,27 +2682,27 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="15365" r:id="rId9" name="btnCreateWorkSheet">
+        <control shapeId="15364" r:id="rId9" name="btnCreatePlanning">
           <controlPr defaultSize="0" autoLine="0" r:id="rId10">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>8</xdr:row>
-                <xdr:rowOff>190500</xdr:rowOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>6</xdr:col>
-                <xdr:colOff>114300</xdr:colOff>
-                <xdr:row>10</xdr:row>
-                <xdr:rowOff>152400</xdr:rowOff>
+                <xdr:colOff>95250</xdr:colOff>
+                <xdr:row>7</xdr:row>
+                <xdr:rowOff>47625</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="15365" r:id="rId9" name="btnCreateWorkSheet"/>
+        <control shapeId="15364" r:id="rId9" name="btnCreatePlanning"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -2729,7 +2741,7 @@
     </row>
     <row r="3" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="19"/>
-      <c r="B3" s="97" t="s">
+      <c r="B3" s="99" t="s">
         <v>21</v>
       </c>
       <c r="C3" s="16">
@@ -2738,7 +2750,7 @@
     </row>
     <row r="4" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="19"/>
-      <c r="B4" s="98"/>
+      <c r="B4" s="100"/>
       <c r="C4" s="22">
         <v>0</v>
       </c>
@@ -3399,7 +3411,7 @@
   <sheetPr codeName="Feuil5"/>
   <dimension ref="A1:H281"/>
   <sheetViews>
-    <sheetView topLeftCell="A64" workbookViewId="0">
+    <sheetView topLeftCell="A67" workbookViewId="0">
       <selection activeCell="C87" sqref="C87"/>
     </sheetView>
   </sheetViews>
@@ -5688,8 +5700,8 @@
   <sheetPr codeName="Feuil9"/>
   <dimension ref="A1:H381"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
-      <selection activeCell="C138" sqref="C138"/>
+    <sheetView tabSelected="1" topLeftCell="A135" workbookViewId="0">
+      <selection activeCell="C156" sqref="C156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -6263,7 +6275,7 @@
       </c>
       <c r="D62" s="10"/>
     </row>
-    <row r="63" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="A63" s="1"/>
       <c r="B63" s="2">
         <v>1</v>
@@ -6838,7 +6850,7 @@
       <c r="B136" s="4">
         <v>2</v>
       </c>
-      <c r="C136" s="99" t="s">
+      <c r="C136" s="95" t="s">
         <v>88</v>
       </c>
       <c r="D136" s="9"/>
@@ -6850,7 +6862,7 @@
       <c r="B137" s="2">
         <v>1</v>
       </c>
-      <c r="C137" s="100" t="s">
+      <c r="C137" s="96" t="s">
         <v>89</v>
       </c>
       <c r="D137" s="10"/>
@@ -6862,7 +6874,7 @@
       <c r="B138" s="2">
         <v>1</v>
       </c>
-      <c r="C138" s="100" t="s">
+      <c r="C138" s="96" t="s">
         <v>91</v>
       </c>
       <c r="D138" s="10"/>
@@ -6988,27 +7000,51 @@
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A155" s="5"/>
-      <c r="B155" s="4"/>
-      <c r="C155" s="9"/>
+      <c r="A155" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B155" s="4">
+        <v>1</v>
+      </c>
+      <c r="C155" s="95" t="s">
+        <v>92</v>
+      </c>
       <c r="D155" s="9"/>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A156" s="1"/>
-      <c r="B156" s="2"/>
-      <c r="C156" s="10"/>
+    <row r="156" spans="1:4" ht="27" x14ac:dyDescent="0.25">
+      <c r="A156" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B156" s="2">
+        <v>1</v>
+      </c>
+      <c r="C156" s="96" t="s">
+        <v>95</v>
+      </c>
       <c r="D156" s="10"/>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A157" s="1"/>
-      <c r="B157" s="2"/>
-      <c r="C157" s="10"/>
+      <c r="A157" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B157" s="2">
+        <v>1</v>
+      </c>
+      <c r="C157" s="96" t="s">
+        <v>93</v>
+      </c>
       <c r="D157" s="10"/>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A158" s="1"/>
-      <c r="B158" s="2"/>
-      <c r="C158" s="10"/>
+      <c r="A158" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B158" s="2">
+        <v>1</v>
+      </c>
+      <c r="C158" s="96" t="s">
+        <v>94</v>
+      </c>
       <c r="D158" s="10"/>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
@@ -7083,7 +7119,7 @@
       </c>
       <c r="B170" s="47">
         <f>SUM(B155:B169)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C170" s="88" t="s">
         <v>34</v>
@@ -8671,26 +8707,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="bf2f2df3-a963-4452-b0e7-67dabc627c35">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="f7d9f5a6-831d-4621-8c77-cbcaf993e406" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001ABD9BFFC9E543439C53A2705AE306EF" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="a2a625e4713a1206e22a4c67b5bce77a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="bf2f2df3-a963-4452-b0e7-67dabc627c35" xmlns:ns3="f7d9f5a6-831d-4621-8c77-cbcaf993e406" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="44987950040cbf76ec9c25f294fcc9dd" ns2:_="" ns3:_="">
     <xsd:import namespace="bf2f2df3-a963-4452-b0e7-67dabc627c35"/>
@@ -8911,10 +8927,41 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="bf2f2df3-a963-4452-b0e7-67dabc627c35">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="f7d9f5a6-831d-4621-8c77-cbcaf993e406" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{483719EA-391A-4C4B-985B-9805B7FCB9D5}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B433C9A-8A3A-4D69-955C-F3F07BFE315A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="bf2f2df3-a963-4452-b0e7-67dabc627c35"/>
+    <ds:schemaRef ds:uri="f7d9f5a6-831d-4621-8c77-cbcaf993e406"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -8931,20 +8978,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B433C9A-8A3A-4D69-955C-F3F07BFE315A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{483719EA-391A-4C4B-985B-9805B7FCB9D5}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="bf2f2df3-a963-4452-b0e7-67dabc627c35"/>
-    <ds:schemaRef ds:uri="f7d9f5a6-831d-4621-8c77-cbcaf993e406"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
j'ai ajouté les murs et les position d'objet est juste et il tire et bouge la même temps
</commit_message>
<xml_diff>
--- a/Docs/planification-Projet-Hanieh Mohajerani.xlsx
+++ b/Docs/planification-Projet-Hanieh Mohajerani.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Cours-Semestre\Semestres\Semestre 1-2\Projet-Module-C#\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CA51BE5-A3AB-4AF6-8272-9958525B319F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E98EFFA2-F9BA-43AD-A146-023C4AF6C1F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="99">
   <si>
     <t>Module :</t>
   </si>
@@ -356,6 +356,15 @@
   </si>
   <si>
     <t>j'ai corrigé les missiles car avant les missiles d'enemie a marché pas juste mais ce n'a pas encore fini</t>
+  </si>
+  <si>
+    <t>créer les petites enemies</t>
+  </si>
+  <si>
+    <t>position random juste</t>
+  </si>
+  <si>
+    <t>créer les missile de petites enemy</t>
   </si>
 </sst>
 </file>
@@ -2632,27 +2641,27 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="15365" r:id="rId5" name="btnCreateWorkSheet">
+        <control shapeId="15364" r:id="rId5" name="btnCreatePlanning">
           <controlPr defaultSize="0" autoLine="0" r:id="rId6">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>8</xdr:row>
-                <xdr:rowOff>190500</xdr:rowOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>6</xdr:col>
-                <xdr:colOff>114300</xdr:colOff>
-                <xdr:row>10</xdr:row>
-                <xdr:rowOff>152400</xdr:rowOff>
+                <xdr:colOff>95250</xdr:colOff>
+                <xdr:row>7</xdr:row>
+                <xdr:rowOff>47625</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="15365" r:id="rId5" name="btnCreateWorkSheet"/>
+        <control shapeId="15364" r:id="rId5" name="btnCreatePlanning"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -2682,27 +2691,27 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="15364" r:id="rId9" name="btnCreatePlanning">
+        <control shapeId="15365" r:id="rId9" name="btnCreateWorkSheet">
           <controlPr defaultSize="0" autoLine="0" r:id="rId10">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>5</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
+                <xdr:row>8</xdr:row>
+                <xdr:rowOff>190500</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>6</xdr:col>
-                <xdr:colOff>95250</xdr:colOff>
-                <xdr:row>7</xdr:row>
-                <xdr:rowOff>47625</xdr:rowOff>
+                <xdr:colOff>114300</xdr:colOff>
+                <xdr:row>10</xdr:row>
+                <xdr:rowOff>152400</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="15364" r:id="rId9" name="btnCreatePlanning"/>
+        <control shapeId="15365" r:id="rId9" name="btnCreateWorkSheet"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -3411,7 +3420,7 @@
   <sheetPr codeName="Feuil5"/>
   <dimension ref="A1:H281"/>
   <sheetViews>
-    <sheetView topLeftCell="A67" workbookViewId="0">
+    <sheetView topLeftCell="A77" workbookViewId="0">
       <selection activeCell="C87" sqref="C87"/>
     </sheetView>
   </sheetViews>
@@ -5700,8 +5709,8 @@
   <sheetPr codeName="Feuil9"/>
   <dimension ref="A1:H381"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A135" workbookViewId="0">
-      <selection activeCell="C156" sqref="C156"/>
+    <sheetView tabSelected="1" topLeftCell="A148" workbookViewId="0">
+      <selection activeCell="B177" sqref="B177"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -7162,21 +7171,39 @@
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A174" s="5"/>
-      <c r="B174" s="4"/>
-      <c r="C174" s="9"/>
+      <c r="A174" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B174" s="4">
+        <v>1</v>
+      </c>
+      <c r="C174" s="95" t="s">
+        <v>96</v>
+      </c>
       <c r="D174" s="9"/>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A175" s="1"/>
-      <c r="B175" s="2"/>
-      <c r="C175" s="10"/>
+      <c r="A175" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B175" s="2">
+        <v>1</v>
+      </c>
+      <c r="C175" s="96" t="s">
+        <v>97</v>
+      </c>
       <c r="D175" s="10"/>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A176" s="1"/>
-      <c r="B176" s="2"/>
-      <c r="C176" s="10"/>
+      <c r="A176" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B176" s="2">
+        <v>2</v>
+      </c>
+      <c r="C176" s="96" t="s">
+        <v>98</v>
+      </c>
       <c r="D176" s="10"/>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
@@ -7257,7 +7284,7 @@
       </c>
       <c r="B189" s="47">
         <f>SUM(B174:B188)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C189" s="88" t="s">
         <v>34</v>
@@ -8707,6 +8734,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="bf2f2df3-a963-4452-b0e7-67dabc627c35">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="f7d9f5a6-831d-4621-8c77-cbcaf993e406" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001ABD9BFFC9E543439C53A2705AE306EF" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="a2a625e4713a1206e22a4c67b5bce77a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="bf2f2df3-a963-4452-b0e7-67dabc627c35" xmlns:ns3="f7d9f5a6-831d-4621-8c77-cbcaf993e406" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="44987950040cbf76ec9c25f294fcc9dd" ns2:_="" ns3:_="">
     <xsd:import namespace="bf2f2df3-a963-4452-b0e7-67dabc627c35"/>
@@ -8927,27 +8974,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="bf2f2df3-a963-4452-b0e7-67dabc627c35">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="f7d9f5a6-831d-4621-8c77-cbcaf993e406" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{483719EA-391A-4C4B-985B-9805B7FCB9D5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7C29126A-0525-4FCA-A870-5924A033DD5A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="bf2f2df3-a963-4452-b0e7-67dabc627c35"/>
+    <ds:schemaRef ds:uri="f7d9f5a6-831d-4621-8c77-cbcaf993e406"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B433C9A-8A3A-4D69-955C-F3F07BFE315A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8964,23 +9010,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7C29126A-0525-4FCA-A870-5924A033DD5A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="bf2f2df3-a963-4452-b0e7-67dabc627c35"/>
-    <ds:schemaRef ds:uri="f7d9f5a6-831d-4621-8c77-cbcaf993e406"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{483719EA-391A-4C4B-985B-9805B7FCB9D5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
j'ai corrigé les code et les petits enemies peut aller a gauche et droit et descend a la fin de tiuche l'écran et ils tirent vers bas
</commit_message>
<xml_diff>
--- a/Docs/planification-Projet-Hanieh Mohajerani.xlsx
+++ b/Docs/planification-Projet-Hanieh Mohajerani.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Cours-Semestre\Semestres\Semestre 1-2\Projet-Module-C#\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E98EFFA2-F9BA-43AD-A146-023C4AF6C1F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09FF2E37-FF04-4403-89A2-2DBC7A31D349}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Donnees" sheetId="7" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="110">
   <si>
     <t>Module :</t>
   </si>
@@ -365,6 +365,39 @@
   </si>
   <si>
     <t>créer les missile de petites enemy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">j'ai mit tout les petits enemis ensemble </t>
+  </si>
+  <si>
+    <t>j'ai corrige encore mes codes les enemis bouge a gauche et droit et il descend a la fin de chaque ligne</t>
+  </si>
+  <si>
+    <t>j'ai commencé de travailler sur les tirer des enemies</t>
+  </si>
+  <si>
+    <t>j'ai corrigeé les codes des missile que peut tire vers bas</t>
+  </si>
+  <si>
+    <t>vacences</t>
+  </si>
+  <si>
+    <t>j'ai travaillé encore sur les enemies qaund il touche les ecran droit il passe le limite</t>
+  </si>
+  <si>
+    <t xml:space="preserve">j'ai corrigé les errors de toucher enemies a droit car il calcule le premiere enemies pour touche l'ecran maitnent il calcule tout les enemies </t>
+  </si>
+  <si>
+    <t xml:space="preserve">j'ai travaillé sur tirer les missiles il tire vers haut </t>
+  </si>
+  <si>
+    <t>les enemie tire vers bas car j'ai corrigé les codes et j'ai change le valwur 1 avec -1 pour y</t>
+  </si>
+  <si>
+    <t>j'ai testé mes codes et il marche bien les tirer des emissiles.</t>
+  </si>
+  <si>
+    <t>j'ai ajouté 1 classe heritage missile que il s'appelle position pour gerrer les position des missile que tire vers bas pour efface le mure</t>
   </si>
 </sst>
 </file>
@@ -2641,27 +2674,27 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="15364" r:id="rId5" name="btnCreatePlanning">
+        <control shapeId="15365" r:id="rId5" name="btnCreateWorkSheet">
           <controlPr defaultSize="0" autoLine="0" r:id="rId6">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>5</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
+                <xdr:row>8</xdr:row>
+                <xdr:rowOff>190500</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>6</xdr:col>
-                <xdr:colOff>95250</xdr:colOff>
-                <xdr:row>7</xdr:row>
-                <xdr:rowOff>47625</xdr:rowOff>
+                <xdr:colOff>114300</xdr:colOff>
+                <xdr:row>10</xdr:row>
+                <xdr:rowOff>152400</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="15364" r:id="rId5" name="btnCreatePlanning"/>
+        <control shapeId="15365" r:id="rId5" name="btnCreateWorkSheet"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -2691,27 +2724,27 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="15365" r:id="rId9" name="btnCreateWorkSheet">
+        <control shapeId="15364" r:id="rId9" name="btnCreatePlanning">
           <controlPr defaultSize="0" autoLine="0" r:id="rId10">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>8</xdr:row>
-                <xdr:rowOff>190500</xdr:rowOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>6</xdr:col>
-                <xdr:colOff>114300</xdr:colOff>
-                <xdr:row>10</xdr:row>
-                <xdr:rowOff>152400</xdr:rowOff>
+                <xdr:colOff>95250</xdr:colOff>
+                <xdr:row>7</xdr:row>
+                <xdr:rowOff>47625</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="15365" r:id="rId9" name="btnCreateWorkSheet"/>
+        <control shapeId="15364" r:id="rId9" name="btnCreatePlanning"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -5709,8 +5742,8 @@
   <sheetPr codeName="Feuil9"/>
   <dimension ref="A1:H381"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A148" workbookViewId="0">
-      <selection activeCell="B177" sqref="B177"/>
+    <sheetView tabSelected="1" topLeftCell="A226" workbookViewId="0">
+      <selection activeCell="C255" sqref="C255"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -7327,27 +7360,51 @@
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A193" s="5"/>
-      <c r="B193" s="4"/>
-      <c r="C193" s="9"/>
+      <c r="A193" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B193" s="4">
+        <v>1</v>
+      </c>
+      <c r="C193" s="95" t="s">
+        <v>99</v>
+      </c>
       <c r="D193" s="9"/>
     </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A194" s="1"/>
-      <c r="B194" s="2"/>
-      <c r="C194" s="10"/>
+    <row r="194" spans="1:4" ht="27" x14ac:dyDescent="0.25">
+      <c r="A194" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B194" s="2">
+        <v>1</v>
+      </c>
+      <c r="C194" s="96" t="s">
+        <v>100</v>
+      </c>
       <c r="D194" s="10"/>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A195" s="1"/>
-      <c r="B195" s="2"/>
-      <c r="C195" s="10"/>
+      <c r="A195" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B195" s="2">
+        <v>1</v>
+      </c>
+      <c r="C195" s="96" t="s">
+        <v>101</v>
+      </c>
       <c r="D195" s="10"/>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A196" s="1"/>
-      <c r="B196" s="2"/>
-      <c r="C196" s="10"/>
+      <c r="A196" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B196" s="2">
+        <v>1</v>
+      </c>
+      <c r="C196" s="96" t="s">
+        <v>102</v>
+      </c>
       <c r="D196" s="10"/>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.25">
@@ -7422,7 +7479,7 @@
       </c>
       <c r="B208" s="47">
         <f>SUM(B193:B207)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C208" s="88" t="s">
         <v>34</v>
@@ -7467,7 +7524,9 @@
     <row r="212" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A212" s="5"/>
       <c r="B212" s="4"/>
-      <c r="C212" s="9"/>
+      <c r="C212" s="95" t="s">
+        <v>82</v>
+      </c>
       <c r="D212" s="9"/>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
@@ -7605,7 +7664,9 @@
     <row r="231" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A231" s="5"/>
       <c r="B231" s="4"/>
-      <c r="C231" s="9"/>
+      <c r="C231" s="95" t="s">
+        <v>103</v>
+      </c>
       <c r="D231" s="9"/>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.25">
@@ -7741,39 +7802,75 @@
       </c>
     </row>
     <row r="250" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A250" s="5"/>
-      <c r="B250" s="4"/>
-      <c r="C250" s="9"/>
+      <c r="A250" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B250" s="4">
+        <v>1</v>
+      </c>
+      <c r="C250" s="95" t="s">
+        <v>104</v>
+      </c>
       <c r="D250" s="9"/>
     </row>
     <row r="251" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A251" s="1"/>
-      <c r="B251" s="2"/>
-      <c r="C251" s="10"/>
+      <c r="A251" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B251" s="2">
+        <v>1</v>
+      </c>
+      <c r="C251" s="96" t="s">
+        <v>106</v>
+      </c>
       <c r="D251" s="10"/>
     </row>
-    <row r="252" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A252" s="1"/>
-      <c r="B252" s="2"/>
-      <c r="C252" s="10"/>
+    <row r="252" spans="1:4" ht="27" x14ac:dyDescent="0.25">
+      <c r="A252" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B252" s="2">
+        <v>1</v>
+      </c>
+      <c r="C252" s="96" t="s">
+        <v>105</v>
+      </c>
       <c r="D252" s="10"/>
     </row>
     <row r="253" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A253" s="1"/>
-      <c r="B253" s="2"/>
-      <c r="C253" s="10"/>
+      <c r="A253" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B253" s="2">
+        <v>1</v>
+      </c>
+      <c r="C253" s="96" t="s">
+        <v>107</v>
+      </c>
       <c r="D253" s="10"/>
     </row>
     <row r="254" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A254" s="1"/>
-      <c r="B254" s="2"/>
-      <c r="C254" s="10"/>
+      <c r="A254" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B254" s="2">
+        <v>1</v>
+      </c>
+      <c r="C254" s="96" t="s">
+        <v>108</v>
+      </c>
       <c r="D254" s="10"/>
     </row>
-    <row r="255" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A255" s="1"/>
-      <c r="B255" s="2"/>
-      <c r="C255" s="10"/>
+    <row r="255" spans="1:4" ht="27" x14ac:dyDescent="0.25">
+      <c r="A255" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B255" s="2">
+        <v>1</v>
+      </c>
+      <c r="C255" s="96" t="s">
+        <v>109</v>
+      </c>
       <c r="D255" s="10"/>
     </row>
     <row r="256" spans="1:4" x14ac:dyDescent="0.25">
@@ -7836,7 +7933,7 @@
       </c>
       <c r="B265" s="47">
         <f>SUM(B250:B264)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C265" s="88" t="s">
         <v>34</v>
@@ -8734,26 +8831,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="bf2f2df3-a963-4452-b0e7-67dabc627c35">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="f7d9f5a6-831d-4621-8c77-cbcaf993e406" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001ABD9BFFC9E543439C53A2705AE306EF" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="a2a625e4713a1206e22a4c67b5bce77a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="bf2f2df3-a963-4452-b0e7-67dabc627c35" xmlns:ns3="f7d9f5a6-831d-4621-8c77-cbcaf993e406" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="44987950040cbf76ec9c25f294fcc9dd" ns2:_="" ns3:_="">
     <xsd:import namespace="bf2f2df3-a963-4452-b0e7-67dabc627c35"/>
@@ -8974,10 +9051,41 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="bf2f2df3-a963-4452-b0e7-67dabc627c35">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="f7d9f5a6-831d-4621-8c77-cbcaf993e406" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{483719EA-391A-4C4B-985B-9805B7FCB9D5}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B433C9A-8A3A-4D69-955C-F3F07BFE315A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="bf2f2df3-a963-4452-b0e7-67dabc627c35"/>
+    <ds:schemaRef ds:uri="f7d9f5a6-831d-4621-8c77-cbcaf993e406"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -8994,20 +9102,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B433C9A-8A3A-4D69-955C-F3F07BFE315A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{483719EA-391A-4C4B-985B-9805B7FCB9D5}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="bf2f2df3-a963-4452-b0e7-67dabc627c35"/>
-    <ds:schemaRef ds:uri="f7d9f5a6-831d-4621-8c77-cbcaf993e406"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
j'ai corriges les error pour toucher le mur par enemies et ca march et il tire vers bas les enemeies par random et j'ai commenc a corriger pour les missile peut effacer le mur
Signed-off-by: Haniehmoh <pl23bay@eduvaud.ch>
</commit_message>
<xml_diff>
--- a/Docs/planification-Projet-Hanieh Mohajerani.xlsx
+++ b/Docs/planification-Projet-Hanieh Mohajerani.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Cours-Semestre\Semestres\Semestre 1-2\Projet-Module-C#\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09FF2E37-FF04-4403-89A2-2DBC7A31D349}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{296A3DA5-09AC-4086-8057-3724066BA925}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Donnees" sheetId="7" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="122">
   <si>
     <t>Module :</t>
   </si>
@@ -398,6 +398,42 @@
   </si>
   <si>
     <t>j'ai ajouté 1 classe heritage missile que il s'appelle position pour gerrer les position des missile que tire vers bas pour efface le mure</t>
+  </si>
+  <si>
+    <t>j'ai continu a travailler sur les misile qand il touche les mur</t>
+  </si>
+  <si>
+    <t>j'ai creé le copie de mon code dans l'autre projet car je puisse modifier les position des ennemis et je missile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">j'ai essayé de corrigé les codes pour effacer les mure mais ca marche pas juste </t>
+  </si>
+  <si>
+    <t>j'ai corrigé les code pour arriver a faire pour chaque enemies un nouveau position mais ca march pas encore</t>
+  </si>
+  <si>
+    <t>j'ai cree 3 vie pour le chip</t>
+  </si>
+  <si>
+    <t>continue a travailler sur les missile et touchant les mures depuis petit enemie et ship et ca marche et juste que j'ai 2 colons pour les mure et je dois corriger</t>
+  </si>
+  <si>
+    <t>travail sur les effacer le ship apres 3 fois toucher  depuis les petit enemies missiles</t>
+  </si>
+  <si>
+    <t>j'ai creé le timer pour 30 second</t>
+  </si>
+  <si>
+    <t>jai travaillé sur le methode haninputenemies pour créer chaque enemies en 1 objet et bougent a gauche et droit just ca marche maitnant mais je dois arriver a les effacer en touchant les missile de ship</t>
+  </si>
+  <si>
+    <t>j'ai trvaillé sur effacer les petites enemies</t>
+  </si>
+  <si>
+    <t xml:space="preserve">j'ai separer le methode créer les enemies et boule et tire en 2 methode et maitnant ca marche créer des enemies mais je trvail sur bouger des enemies </t>
+  </si>
+  <si>
+    <t>jai travaillé sur rirer des enemies que ca marche il rest just  bouger des enemies que ca marche pas bien n</t>
   </si>
 </sst>
 </file>
@@ -2663,7 +2699,7 @@
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="57" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="52" orientation="landscape" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;L&amp;"ETML L,Normal"ETML&amp;C&amp;"-,Normal"Planification&amp;R&amp;G</oddHeader>
     <oddFooter>&amp;L&amp;"-,Normal"&amp;D - GGZ&amp;C&amp;"-,Normal"&amp;F - &amp;A&amp;R&amp;"-,Normal"Page &amp;P/&amp;N</oddFooter>
@@ -2674,27 +2710,27 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="15365" r:id="rId5" name="btnCreateWorkSheet">
+        <control shapeId="15364" r:id="rId5" name="btnCreatePlanning">
           <controlPr defaultSize="0" autoLine="0" r:id="rId6">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>8</xdr:row>
-                <xdr:rowOff>190500</xdr:rowOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>6</xdr:col>
-                <xdr:colOff>114300</xdr:colOff>
-                <xdr:row>10</xdr:row>
-                <xdr:rowOff>152400</xdr:rowOff>
+                <xdr:colOff>95250</xdr:colOff>
+                <xdr:row>7</xdr:row>
+                <xdr:rowOff>47625</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="15365" r:id="rId5" name="btnCreateWorkSheet"/>
+        <control shapeId="15364" r:id="rId5" name="btnCreatePlanning"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -2724,27 +2760,27 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="15364" r:id="rId9" name="btnCreatePlanning">
+        <control shapeId="15365" r:id="rId9" name="btnCreateWorkSheet">
           <controlPr defaultSize="0" autoLine="0" r:id="rId10">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>5</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
+                <xdr:row>8</xdr:row>
+                <xdr:rowOff>190500</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>6</xdr:col>
-                <xdr:colOff>95250</xdr:colOff>
-                <xdr:row>7</xdr:row>
-                <xdr:rowOff>47625</xdr:rowOff>
+                <xdr:colOff>114300</xdr:colOff>
+                <xdr:row>10</xdr:row>
+                <xdr:rowOff>152400</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="15364" r:id="rId9" name="btnCreatePlanning"/>
+        <control shapeId="15365" r:id="rId9" name="btnCreateWorkSheet"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -5742,8 +5778,8 @@
   <sheetPr codeName="Feuil9"/>
   <dimension ref="A1:H381"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A226" workbookViewId="0">
-      <selection activeCell="C255" sqref="C255"/>
+    <sheetView tabSelected="1" topLeftCell="A319" workbookViewId="0">
+      <selection activeCell="C329" sqref="C329"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -7976,27 +8012,51 @@
       </c>
     </row>
     <row r="269" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A269" s="5"/>
-      <c r="B269" s="4"/>
-      <c r="C269" s="9"/>
+      <c r="A269" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B269" s="4">
+        <v>1</v>
+      </c>
+      <c r="C269" s="95" t="s">
+        <v>110</v>
+      </c>
       <c r="D269" s="9"/>
     </row>
-    <row r="270" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A270" s="1"/>
-      <c r="B270" s="2"/>
-      <c r="C270" s="10"/>
+    <row r="270" spans="1:4" ht="27" x14ac:dyDescent="0.25">
+      <c r="A270" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B270" s="2">
+        <v>1</v>
+      </c>
+      <c r="C270" s="96" t="s">
+        <v>111</v>
+      </c>
       <c r="D270" s="10"/>
     </row>
-    <row r="271" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A271" s="1"/>
-      <c r="B271" s="2"/>
-      <c r="C271" s="10"/>
+    <row r="271" spans="1:4" ht="27" x14ac:dyDescent="0.25">
+      <c r="A271" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B271" s="2">
+        <v>2</v>
+      </c>
+      <c r="C271" s="96" t="s">
+        <v>113</v>
+      </c>
       <c r="D271" s="10"/>
     </row>
     <row r="272" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A272" s="1"/>
-      <c r="B272" s="2"/>
-      <c r="C272" s="10"/>
+      <c r="A272" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B272" s="2">
+        <v>2</v>
+      </c>
+      <c r="C272" s="96" t="s">
+        <v>112</v>
+      </c>
       <c r="D272" s="10"/>
     </row>
     <row r="273" spans="1:4" x14ac:dyDescent="0.25">
@@ -8071,7 +8131,7 @@
       </c>
       <c r="B284" s="47">
         <f>SUM(B269:B283)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C284" s="88" t="s">
         <v>34</v>
@@ -8113,28 +8173,52 @@
         <v>13</v>
       </c>
     </row>
-    <row r="288" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A288" s="5"/>
-      <c r="B288" s="4"/>
-      <c r="C288" s="9"/>
+    <row r="288" spans="1:4" ht="27" x14ac:dyDescent="0.25">
+      <c r="A288" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B288" s="4">
+        <v>3</v>
+      </c>
+      <c r="C288" s="95" t="s">
+        <v>115</v>
+      </c>
       <c r="D288" s="9"/>
     </row>
     <row r="289" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A289" s="1"/>
-      <c r="B289" s="2"/>
-      <c r="C289" s="10"/>
+      <c r="A289" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B289" s="2">
+        <v>1</v>
+      </c>
+      <c r="C289" s="96" t="s">
+        <v>114</v>
+      </c>
       <c r="D289" s="10"/>
     </row>
     <row r="290" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A290" s="1"/>
-      <c r="B290" s="2"/>
-      <c r="C290" s="10"/>
+      <c r="A290" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B290" s="2">
+        <v>2</v>
+      </c>
+      <c r="C290" s="96" t="s">
+        <v>116</v>
+      </c>
       <c r="D290" s="10"/>
     </row>
     <row r="291" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A291" s="1"/>
-      <c r="B291" s="2"/>
-      <c r="C291" s="10"/>
+      <c r="A291" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B291" s="2">
+        <v>1</v>
+      </c>
+      <c r="C291" s="96" t="s">
+        <v>117</v>
+      </c>
       <c r="D291" s="10"/>
     </row>
     <row r="292" spans="1:4" x14ac:dyDescent="0.25">
@@ -8209,7 +8293,7 @@
       </c>
       <c r="B303" s="47">
         <f>SUM(B288:B302)</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="C303" s="88" t="s">
         <v>34</v>
@@ -8254,7 +8338,9 @@
     <row r="307" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A307" s="5"/>
       <c r="B307" s="4"/>
-      <c r="C307" s="9"/>
+      <c r="C307" s="95" t="s">
+        <v>80</v>
+      </c>
       <c r="D307" s="9"/>
     </row>
     <row r="308" spans="1:4" x14ac:dyDescent="0.25">
@@ -8389,28 +8475,52 @@
         <v>13</v>
       </c>
     </row>
-    <row r="326" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A326" s="5"/>
-      <c r="B326" s="4"/>
-      <c r="C326" s="9"/>
+    <row r="326" spans="1:4" ht="40.5" x14ac:dyDescent="0.25">
+      <c r="A326" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B326" s="4">
+        <v>2</v>
+      </c>
+      <c r="C326" s="95" t="s">
+        <v>118</v>
+      </c>
       <c r="D326" s="9"/>
     </row>
     <row r="327" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A327" s="1"/>
-      <c r="B327" s="2"/>
-      <c r="C327" s="10"/>
+      <c r="A327" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B327" s="2">
+        <v>2</v>
+      </c>
+      <c r="C327" s="96" t="s">
+        <v>119</v>
+      </c>
       <c r="D327" s="10"/>
     </row>
-    <row r="328" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A328" s="1"/>
-      <c r="B328" s="2"/>
-      <c r="C328" s="10"/>
+    <row r="328" spans="1:4" ht="27" x14ac:dyDescent="0.25">
+      <c r="A328" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B328" s="2">
+        <v>2</v>
+      </c>
+      <c r="C328" s="96" t="s">
+        <v>120</v>
+      </c>
       <c r="D328" s="10"/>
     </row>
-    <row r="329" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A329" s="1"/>
-      <c r="B329" s="2"/>
-      <c r="C329" s="10"/>
+    <row r="329" spans="1:4" ht="27" x14ac:dyDescent="0.25">
+      <c r="A329" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B329" s="2">
+        <v>1</v>
+      </c>
+      <c r="C329" s="96" t="s">
+        <v>121</v>
+      </c>
       <c r="D329" s="10"/>
     </row>
     <row r="330" spans="1:4" x14ac:dyDescent="0.25">
@@ -8485,7 +8595,7 @@
       </c>
       <c r="B341" s="47">
         <f>SUM(B326:B340)</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="C341" s="88" t="s">
         <v>34</v>
@@ -8831,6 +8941,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="bf2f2df3-a963-4452-b0e7-67dabc627c35">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="f7d9f5a6-831d-4621-8c77-cbcaf993e406" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001ABD9BFFC9E543439C53A2705AE306EF" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="a2a625e4713a1206e22a4c67b5bce77a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="bf2f2df3-a963-4452-b0e7-67dabc627c35" xmlns:ns3="f7d9f5a6-831d-4621-8c77-cbcaf993e406" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="44987950040cbf76ec9c25f294fcc9dd" ns2:_="" ns3:_="">
     <xsd:import namespace="bf2f2df3-a963-4452-b0e7-67dabc627c35"/>
@@ -9051,27 +9181,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="bf2f2df3-a963-4452-b0e7-67dabc627c35">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="f7d9f5a6-831d-4621-8c77-cbcaf993e406" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{483719EA-391A-4C4B-985B-9805B7FCB9D5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7C29126A-0525-4FCA-A870-5924A033DD5A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="bf2f2df3-a963-4452-b0e7-67dabc627c35"/>
+    <ds:schemaRef ds:uri="f7d9f5a6-831d-4621-8c77-cbcaf993e406"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B433C9A-8A3A-4D69-955C-F3F07BFE315A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9088,23 +9217,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7C29126A-0525-4FCA-A870-5924A033DD5A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="bf2f2df3-a963-4452-b0e7-67dabc627c35"/>
-    <ds:schemaRef ds:uri="f7d9f5a6-831d-4621-8c77-cbcaf993e406"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{483719EA-391A-4C4B-985B-9805B7FCB9D5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
j'ai ajouté la diagramme de classe
</commit_message>
<xml_diff>
--- a/Docs/planification-Projet-Hanieh Mohajerani.xlsx
+++ b/Docs/planification-Projet-Hanieh Mohajerani.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Cours-Semestre\Semestres\Semestre 1-2\Projet-Module-C#\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{296A3DA5-09AC-4086-8057-3724066BA925}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{398949A9-2333-4B1F-8545-4B31948105AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Donnees" sheetId="7" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="129">
   <si>
     <t>Module :</t>
   </si>
@@ -250,39 +250,15 @@
     <t>j'ai analyser le sujet,ce n'est pas encore claire pour moi</t>
   </si>
   <si>
-    <t>j'ai regardé sir le site et j'essaie a comprendre mieux</t>
-  </si>
-  <si>
-    <t>j'ai fait le planification pour durée de travail</t>
-  </si>
-  <si>
     <t>créer git hub</t>
   </si>
   <si>
-    <t>j'ai créé mon git hub</t>
-  </si>
-  <si>
-    <t>j'ai creé les methodes et la class  Vecteur2d et la classe SpaceShip,classe game ,ballequitombe et gameobjet et ses methodes dedans</t>
-  </si>
-  <si>
     <t xml:space="preserve"> depelacer le jeu vers le bas </t>
   </si>
   <si>
     <t>depelacer le jeu a gouche et droit</t>
   </si>
   <si>
-    <t xml:space="preserve">j'ai ajouter un champ playerShip de type SpaceShip </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ajoutez le nouveau vaisseau à la liste des objets du jeu.</t>
-  </si>
-  <si>
-    <t>s la méthode Update de la classe SpaceShip</t>
-  </si>
-  <si>
-    <t>j'ai corrigé les codes et ca march,il va a gouche et droit juste.</t>
-  </si>
-  <si>
     <t>depelacment juste a gouche et droit</t>
   </si>
   <si>
@@ -424,9 +400,6 @@
     <t>j'ai creé le timer pour 30 second</t>
   </si>
   <si>
-    <t>jai travaillé sur le methode haninputenemies pour créer chaque enemies en 1 objet et bougent a gauche et droit just ca marche maitnant mais je dois arriver a les effacer en touchant les missile de ship</t>
-  </si>
-  <si>
     <t>j'ai trvaillé sur effacer les petites enemies</t>
   </si>
   <si>
@@ -434,6 +407,54 @@
   </si>
   <si>
     <t>jai travaillé sur rirer des enemies que ca marche il rest just  bouger des enemies que ca marche pas bien n</t>
+  </si>
+  <si>
+    <t>j'ai creé le rapport de projet et corrigé encore les commentaire et diagramme des class</t>
+  </si>
+  <si>
+    <t>j'a ajouté le menu d'entrer dans 1 class separer</t>
+  </si>
+  <si>
+    <t>j'ai testé mes codes avec test unitaire mais le problem ce que je n'ai pas creé ce projet avec MVC dons je ne peux pas tester les méthodes que ils affichent quel qule chose. J'ai testé que les stractures</t>
+  </si>
+  <si>
+    <t>j'ai des problemes sur mes codes par exemple affichache de moment GameOver ou qaund des enemis bougent vers la gauche je ne peux bien les effacer .</t>
+  </si>
+  <si>
+    <t>jai travaillé sur le methode handinputenemies pour créer chaque enemies en 1 objet et bougent a gauche et droit just ca marche maitnant mais je dois arriver a les effacer en touchant les missile de ship</t>
+  </si>
+  <si>
+    <t>j'ai séparé le méthodes HandInputenemies et j'ai creé les autres méthodes comme :CreatEnemies et MoveEnemiesVerticaly MoveAndShootWithEnemies comme ca je peux effacer des enemies depuis mon ship avec tirer des missiles</t>
+  </si>
+  <si>
+    <t>J'ai regardé sur le site et j'essaie de mieux comprendre.</t>
+  </si>
+  <si>
+    <t>J'ai créé mon GitHub</t>
+  </si>
+  <si>
+    <t>J'ai fait la planification pour la durée de travail.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	J'ai corrigé les codes, maintenant le vaisseau se déplace correctement vers la gauche et la droite</t>
+  </si>
+  <si>
+    <t>j'ai créé la classe Missile a fin que je peux créer les methodes pour tirer depuis de mon  vaisseau</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> j'a ajouté le nouveau vaisseau à la liste des objets du jeu.</t>
+  </si>
+  <si>
+    <t>j'ai ajouté la méthode Draw de la classe SpaceShip pour aficher mon vaisseau.</t>
+  </si>
+  <si>
+    <t>. Dans la classe SpaceShip j'ai créé des méthodes pour bouger  mon vaisseau  mais il bouge pas maitnant.le méthode est HandleShipInput.(pas terminé).</t>
+  </si>
+  <si>
+    <t>J'ai créé les méthodes et  les classes SpaceShip, Enemy, avec leurs méthodes</t>
+  </si>
+  <si>
+    <t>j'ai ajouté la condition  dans la méthode Draw pour aficher le  vaisseau</t>
   </si>
 </sst>
 </file>
@@ -2710,27 +2731,27 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="15364" r:id="rId5" name="btnCreatePlanning">
+        <control shapeId="15365" r:id="rId5" name="btnCreateWorkSheet">
           <controlPr defaultSize="0" autoLine="0" r:id="rId6">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>5</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
+                <xdr:row>8</xdr:row>
+                <xdr:rowOff>190500</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>6</xdr:col>
-                <xdr:colOff>95250</xdr:colOff>
-                <xdr:row>7</xdr:row>
-                <xdr:rowOff>47625</xdr:rowOff>
+                <xdr:colOff>114300</xdr:colOff>
+                <xdr:row>10</xdr:row>
+                <xdr:rowOff>152400</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="15364" r:id="rId5" name="btnCreatePlanning"/>
+        <control shapeId="15365" r:id="rId5" name="btnCreateWorkSheet"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -2760,27 +2781,27 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="15365" r:id="rId9" name="btnCreateWorkSheet">
+        <control shapeId="15364" r:id="rId9" name="btnCreatePlanning">
           <controlPr defaultSize="0" autoLine="0" r:id="rId10">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>8</xdr:row>
-                <xdr:rowOff>190500</xdr:rowOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>6</xdr:col>
-                <xdr:colOff>114300</xdr:colOff>
-                <xdr:row>10</xdr:row>
-                <xdr:rowOff>152400</xdr:rowOff>
+                <xdr:colOff>95250</xdr:colOff>
+                <xdr:row>7</xdr:row>
+                <xdr:rowOff>47625</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="15365" r:id="rId9" name="btnCreateWorkSheet"/>
+        <control shapeId="15364" r:id="rId9" name="btnCreatePlanning"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -3489,7 +3510,7 @@
   <sheetPr codeName="Feuil5"/>
   <dimension ref="A1:H281"/>
   <sheetViews>
-    <sheetView topLeftCell="A77" workbookViewId="0">
+    <sheetView topLeftCell="A125" workbookViewId="0">
       <selection activeCell="C87" sqref="C87"/>
     </sheetView>
   </sheetViews>
@@ -3580,7 +3601,7 @@
         <v>1</v>
       </c>
       <c r="C7" s="90" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D7" s="10"/>
     </row>
@@ -3693,7 +3714,7 @@
         <v>2</v>
       </c>
       <c r="C19" s="90" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D19" s="10"/>
     </row>
@@ -3701,7 +3722,7 @@
       <c r="A20" s="1"/>
       <c r="B20" s="2"/>
       <c r="C20" s="90" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D20" s="10"/>
       <c r="F20" s="31"/>
@@ -3844,7 +3865,7 @@
         <v>2</v>
       </c>
       <c r="C33" s="90" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="D33" s="10"/>
     </row>
@@ -3856,7 +3877,7 @@
         <v>1</v>
       </c>
       <c r="C34" s="90" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="D34" s="10"/>
     </row>
@@ -3943,7 +3964,7 @@
       <c r="A45" s="5"/>
       <c r="B45" s="4"/>
       <c r="C45" s="91" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="D45" s="9"/>
     </row>
@@ -3953,7 +3974,7 @@
         <v>2</v>
       </c>
       <c r="C46" s="90" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="D46" s="10"/>
     </row>
@@ -3963,7 +3984,7 @@
         <v>2</v>
       </c>
       <c r="C47" s="90" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="D47" s="10"/>
     </row>
@@ -4056,7 +4077,7 @@
       <c r="A59" s="5"/>
       <c r="B59" s="4"/>
       <c r="C59" s="91" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="D59" s="9"/>
     </row>
@@ -4161,7 +4182,7 @@
       <c r="A73" s="5"/>
       <c r="B73" s="4"/>
       <c r="C73" s="91" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="D73" s="9"/>
     </row>
@@ -4173,7 +4194,7 @@
         <v>2</v>
       </c>
       <c r="C74" s="90" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="D74" s="10"/>
     </row>
@@ -4272,7 +4293,7 @@
       <c r="A87" s="5"/>
       <c r="B87" s="4"/>
       <c r="C87" s="91" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="D87" s="9"/>
     </row>
@@ -5778,8 +5799,8 @@
   <sheetPr codeName="Feuil9"/>
   <dimension ref="A1:H381"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A319" workbookViewId="0">
-      <selection activeCell="C329" sqref="C329"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -5840,7 +5861,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="90" t="s">
-        <v>60</v>
+        <v>119</v>
       </c>
       <c r="D4" s="10"/>
     </row>
@@ -5849,10 +5870,10 @@
         <v>29</v>
       </c>
       <c r="B5" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C5" s="52" t="s">
-        <v>63</v>
+        <v>120</v>
       </c>
       <c r="D5" s="10"/>
     </row>
@@ -5861,26 +5882,35 @@
         <v>28</v>
       </c>
       <c r="B6" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C6" s="90" t="s">
-        <v>61</v>
+        <v>121</v>
       </c>
       <c r="D6" s="10"/>
     </row>
     <row r="7" spans="1:4" s="52" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
+      <c r="A7" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="B7" s="2">
-        <v>1</v>
-      </c>
-      <c r="C7" s="90" t="s">
-        <v>64</v>
+        <v>2</v>
+      </c>
+      <c r="C7" s="52" t="s">
+        <v>127</v>
       </c>
       <c r="D7" s="10"/>
     </row>
-    <row r="8" spans="1:4" s="52" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="2"/>
+    <row r="8" spans="1:4" s="52" customFormat="1" ht="27" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="2">
+        <v>2</v>
+      </c>
+      <c r="C8" s="90" t="s">
+        <v>126</v>
+      </c>
       <c r="D8" s="10"/>
     </row>
     <row r="9" spans="1:4" s="52" customFormat="1" x14ac:dyDescent="0.25">
@@ -5943,7 +5973,7 @@
       </c>
       <c r="B18" s="47">
         <f>SUM(B3:B17)</f>
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C18" s="88" t="s">
         <v>34</v>
@@ -5991,15 +6021,15 @@
       <c r="C22" s="9"/>
       <c r="D22" s="9"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="27" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B23" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C23" s="90" t="s">
-        <v>67</v>
+        <v>123</v>
       </c>
       <c r="D23" s="10"/>
     </row>
@@ -6008,20 +6038,22 @@
         <v>28</v>
       </c>
       <c r="B24" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C24" s="90" t="s">
-        <v>68</v>
+        <v>124</v>
       </c>
       <c r="D24" s="10"/>
     </row>
     <row r="25" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="1"/>
+      <c r="A25" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="B25" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C25" s="90" t="s">
-        <v>69</v>
+        <v>125</v>
       </c>
       <c r="D25" s="10"/>
       <c r="F25" s="31"/>
@@ -6029,9 +6061,15 @@
       <c r="H25" s="33"/>
     </row>
     <row r="26" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A26" s="1"/>
-      <c r="B26" s="2"/>
-      <c r="C26" s="10"/>
+      <c r="A26" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B26" s="2">
+        <v>2</v>
+      </c>
+      <c r="C26" s="96" t="s">
+        <v>128</v>
+      </c>
       <c r="D26" s="10"/>
       <c r="F26" s="34"/>
       <c r="G26" s="30"/>
@@ -6133,7 +6171,7 @@
       </c>
       <c r="B37" s="47">
         <f>SUM(B22:B36)</f>
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C37" s="88" t="s">
         <v>34</v>
@@ -6181,15 +6219,15 @@
       <c r="C41" s="9"/>
       <c r="D41" s="9"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" ht="27" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B42" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C42" s="90" t="s">
-        <v>70</v>
+        <v>122</v>
       </c>
       <c r="D42" s="10"/>
     </row>
@@ -6199,7 +6237,7 @@
         <v>1</v>
       </c>
       <c r="C43" s="90" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="D43" s="10"/>
     </row>
@@ -6281,7 +6319,7 @@
       </c>
       <c r="B56" s="47">
         <f>SUM(B41:B55)</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C56" s="88" t="s">
         <v>34</v>
@@ -6337,7 +6375,7 @@
         <v>2</v>
       </c>
       <c r="C61" s="90" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="D61" s="10"/>
     </row>
@@ -6349,7 +6387,7 @@
         <v>1</v>
       </c>
       <c r="C62" s="90" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="D62" s="10"/>
     </row>
@@ -6359,7 +6397,7 @@
         <v>1</v>
       </c>
       <c r="C63" s="94" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="D63" s="10"/>
     </row>
@@ -6481,7 +6519,7 @@
       <c r="A79" s="5"/>
       <c r="B79" s="4"/>
       <c r="C79" s="91" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="D79" s="9"/>
     </row>
@@ -6625,7 +6663,7 @@
         <v>2</v>
       </c>
       <c r="C98" s="91" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="D98" s="9"/>
     </row>
@@ -6773,7 +6811,7 @@
         <v>2</v>
       </c>
       <c r="C117" s="91" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="D117" s="9"/>
     </row>
@@ -6785,7 +6823,7 @@
         <v>1</v>
       </c>
       <c r="C118" s="90" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="D118" s="10"/>
     </row>
@@ -6797,7 +6835,7 @@
         <v>1</v>
       </c>
       <c r="C119" s="90" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="D119" s="10"/>
     </row>
@@ -6929,7 +6967,7 @@
         <v>2</v>
       </c>
       <c r="C136" s="95" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="D136" s="9"/>
     </row>
@@ -6941,7 +6979,7 @@
         <v>1</v>
       </c>
       <c r="C137" s="96" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="D137" s="10"/>
     </row>
@@ -6953,7 +6991,7 @@
         <v>1</v>
       </c>
       <c r="C138" s="96" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="D138" s="10"/>
     </row>
@@ -7085,7 +7123,7 @@
         <v>1</v>
       </c>
       <c r="C155" s="95" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="D155" s="9"/>
     </row>
@@ -7097,7 +7135,7 @@
         <v>1</v>
       </c>
       <c r="C156" s="96" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="D156" s="10"/>
     </row>
@@ -7109,7 +7147,7 @@
         <v>1</v>
       </c>
       <c r="C157" s="96" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="D157" s="10"/>
     </row>
@@ -7121,7 +7159,7 @@
         <v>1</v>
       </c>
       <c r="C158" s="96" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="D158" s="10"/>
     </row>
@@ -7247,7 +7285,7 @@
         <v>1</v>
       </c>
       <c r="C174" s="95" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="D174" s="9"/>
     </row>
@@ -7259,7 +7297,7 @@
         <v>1</v>
       </c>
       <c r="C175" s="96" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="D175" s="10"/>
     </row>
@@ -7271,7 +7309,7 @@
         <v>2</v>
       </c>
       <c r="C176" s="96" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="D176" s="10"/>
     </row>
@@ -7403,7 +7441,7 @@
         <v>1</v>
       </c>
       <c r="C193" s="95" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="D193" s="9"/>
     </row>
@@ -7415,7 +7453,7 @@
         <v>1</v>
       </c>
       <c r="C194" s="96" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="D194" s="10"/>
     </row>
@@ -7427,7 +7465,7 @@
         <v>1</v>
       </c>
       <c r="C195" s="96" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="D195" s="10"/>
     </row>
@@ -7439,7 +7477,7 @@
         <v>1</v>
       </c>
       <c r="C196" s="96" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="D196" s="10"/>
     </row>
@@ -7561,7 +7599,7 @@
       <c r="A212" s="5"/>
       <c r="B212" s="4"/>
       <c r="C212" s="95" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="D212" s="9"/>
     </row>
@@ -7701,7 +7739,7 @@
       <c r="A231" s="5"/>
       <c r="B231" s="4"/>
       <c r="C231" s="95" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="D231" s="9"/>
     </row>
@@ -7842,10 +7880,10 @@
         <v>28</v>
       </c>
       <c r="B250" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C250" s="95" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="D250" s="9"/>
     </row>
@@ -7854,10 +7892,10 @@
         <v>28</v>
       </c>
       <c r="B251" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C251" s="96" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="D251" s="10"/>
     </row>
@@ -7866,10 +7904,10 @@
         <v>28</v>
       </c>
       <c r="B252" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C252" s="96" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="D252" s="10"/>
     </row>
@@ -7878,10 +7916,10 @@
         <v>28</v>
       </c>
       <c r="B253" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C253" s="96" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="D253" s="10"/>
     </row>
@@ -7893,7 +7931,7 @@
         <v>1</v>
       </c>
       <c r="C254" s="96" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="D254" s="10"/>
     </row>
@@ -7902,10 +7940,10 @@
         <v>28</v>
       </c>
       <c r="B255" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C255" s="96" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="D255" s="10"/>
     </row>
@@ -7969,7 +8007,7 @@
       </c>
       <c r="B265" s="47">
         <f>SUM(B250:B264)</f>
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C265" s="88" t="s">
         <v>34</v>
@@ -8016,10 +8054,10 @@
         <v>28</v>
       </c>
       <c r="B269" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C269" s="95" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="D269" s="9"/>
     </row>
@@ -8028,10 +8066,10 @@
         <v>28</v>
       </c>
       <c r="B270" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C270" s="96" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="D270" s="10"/>
     </row>
@@ -8043,7 +8081,7 @@
         <v>2</v>
       </c>
       <c r="C271" s="96" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="D271" s="10"/>
     </row>
@@ -8055,7 +8093,7 @@
         <v>2</v>
       </c>
       <c r="C272" s="96" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="D272" s="10"/>
     </row>
@@ -8131,7 +8169,7 @@
       </c>
       <c r="B284" s="47">
         <f>SUM(B269:B283)</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C284" s="88" t="s">
         <v>34</v>
@@ -8181,7 +8219,7 @@
         <v>3</v>
       </c>
       <c r="C288" s="95" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="D288" s="9"/>
     </row>
@@ -8190,10 +8228,10 @@
         <v>28</v>
       </c>
       <c r="B289" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C289" s="96" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="D289" s="10"/>
     </row>
@@ -8205,7 +8243,7 @@
         <v>2</v>
       </c>
       <c r="C290" s="96" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="D290" s="10"/>
     </row>
@@ -8214,10 +8252,10 @@
         <v>28</v>
       </c>
       <c r="B291" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C291" s="96" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="D291" s="10"/>
     </row>
@@ -8293,7 +8331,7 @@
       </c>
       <c r="B303" s="47">
         <f>SUM(B288:B302)</f>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C303" s="88" t="s">
         <v>34</v>
@@ -8339,7 +8377,7 @@
       <c r="A307" s="5"/>
       <c r="B307" s="4"/>
       <c r="C307" s="95" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="D307" s="9"/>
     </row>
@@ -8483,7 +8521,7 @@
         <v>2</v>
       </c>
       <c r="C326" s="95" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D326" s="9"/>
     </row>
@@ -8495,7 +8533,7 @@
         <v>2</v>
       </c>
       <c r="C327" s="96" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="D327" s="10"/>
     </row>
@@ -8507,7 +8545,7 @@
         <v>2</v>
       </c>
       <c r="C328" s="96" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="D328" s="10"/>
     </row>
@@ -8519,14 +8557,16 @@
         <v>1</v>
       </c>
       <c r="C329" s="96" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="D329" s="10"/>
     </row>
-    <row r="330" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:4" ht="40.5" x14ac:dyDescent="0.25">
       <c r="A330" s="1"/>
       <c r="B330" s="2"/>
-      <c r="C330" s="10"/>
+      <c r="C330" s="96" t="s">
+        <v>118</v>
+      </c>
       <c r="D330" s="10"/>
     </row>
     <row r="331" spans="1:4" x14ac:dyDescent="0.25">
@@ -8638,27 +8678,51 @@
       </c>
     </row>
     <row r="345" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A345" s="5"/>
-      <c r="B345" s="4"/>
-      <c r="C345" s="9"/>
+      <c r="A345" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B345" s="4">
+        <v>4</v>
+      </c>
+      <c r="C345" s="95" t="s">
+        <v>113</v>
+      </c>
       <c r="D345" s="9"/>
     </row>
     <row r="346" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A346" s="1"/>
-      <c r="B346" s="2"/>
-      <c r="C346" s="10"/>
+      <c r="A346" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B346" s="2">
+        <v>2</v>
+      </c>
+      <c r="C346" s="96" t="s">
+        <v>114</v>
+      </c>
       <c r="D346" s="10"/>
     </row>
-    <row r="347" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A347" s="1"/>
-      <c r="B347" s="2"/>
-      <c r="C347" s="10"/>
+    <row r="347" spans="1:4" ht="40.5" x14ac:dyDescent="0.25">
+      <c r="A347" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B347" s="2">
+        <v>2</v>
+      </c>
+      <c r="C347" s="96" t="s">
+        <v>115</v>
+      </c>
       <c r="D347" s="10"/>
     </row>
-    <row r="348" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A348" s="1"/>
-      <c r="B348" s="2"/>
-      <c r="C348" s="10"/>
+    <row r="348" spans="1:4" ht="27" x14ac:dyDescent="0.25">
+      <c r="A348" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B348" s="2">
+        <v>2</v>
+      </c>
+      <c r="C348" s="96" t="s">
+        <v>116</v>
+      </c>
       <c r="D348" s="10"/>
     </row>
     <row r="349" spans="1:4" x14ac:dyDescent="0.25">
@@ -8733,7 +8797,7 @@
       </c>
       <c r="B360" s="47">
         <f>SUM(B345:B359)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C360" s="88" t="s">
         <v>34</v>
@@ -8776,9 +8840,9 @@
       </c>
     </row>
     <row r="364" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A364" s="5"/>
-      <c r="B364" s="4"/>
-      <c r="C364" s="9"/>
+      <c r="A364" s="1"/>
+      <c r="B364" s="2"/>
+      <c r="C364" s="10"/>
       <c r="D364" s="9"/>
     </row>
     <row r="365" spans="1:4" x14ac:dyDescent="0.25">
@@ -8830,7 +8894,7 @@
       <c r="D372" s="10"/>
     </row>
     <row r="373" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A373" s="2"/>
+      <c r="A373" s="1"/>
       <c r="B373" s="2"/>
       <c r="C373" s="10"/>
       <c r="D373" s="10"/>
@@ -8870,8 +8934,8 @@
         <v>22</v>
       </c>
       <c r="B379" s="47">
-        <f>SUM(B364:B378)</f>
-        <v>0</v>
+        <f>SUM(B345:B378)</f>
+        <v>40</v>
       </c>
       <c r="C379" s="88" t="s">
         <v>34</v>
@@ -8941,26 +9005,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="bf2f2df3-a963-4452-b0e7-67dabc627c35">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="f7d9f5a6-831d-4621-8c77-cbcaf993e406" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001ABD9BFFC9E543439C53A2705AE306EF" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="a2a625e4713a1206e22a4c67b5bce77a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="bf2f2df3-a963-4452-b0e7-67dabc627c35" xmlns:ns3="f7d9f5a6-831d-4621-8c77-cbcaf993e406" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="44987950040cbf76ec9c25f294fcc9dd" ns2:_="" ns3:_="">
     <xsd:import namespace="bf2f2df3-a963-4452-b0e7-67dabc627c35"/>
@@ -9181,10 +9225,41 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="bf2f2df3-a963-4452-b0e7-67dabc627c35">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="f7d9f5a6-831d-4621-8c77-cbcaf993e406" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{483719EA-391A-4C4B-985B-9805B7FCB9D5}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B433C9A-8A3A-4D69-955C-F3F07BFE315A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="bf2f2df3-a963-4452-b0e7-67dabc627c35"/>
+    <ds:schemaRef ds:uri="f7d9f5a6-831d-4621-8c77-cbcaf993e406"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -9201,20 +9276,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B433C9A-8A3A-4D69-955C-F3F07BFE315A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{483719EA-391A-4C4B-985B-9805B7FCB9D5}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="bf2f2df3-a963-4452-b0e7-67dabc627c35"/>
-    <ds:schemaRef ds:uri="f7d9f5a6-831d-4621-8c77-cbcaf993e406"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>